<commit_message>
Added new field to users
ProfileImageUrl varchar(100) not null
</commit_message>
<xml_diff>
--- a/Docs/Adatbázis/Modellek gyűjteménye.xlsx
+++ b/Docs/Adatbázis/Modellek gyűjteménye.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\House of Swords\gameszko\Docs\Adatbázis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822CB9ED-DB05-469E-85F6-AAD6CA6F2ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4695E6-2415-4385-B6D3-2D47B1477BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="254">
   <si>
     <t>User</t>
   </si>
@@ -86,9 +86,6 @@
     <t>PwdHash</t>
   </si>
   <si>
-    <t>max 128, rejtett</t>
-  </si>
-  <si>
     <t>""</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>PwdSalt</t>
   </si>
   <si>
-    <t>max 20, rejtett</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -122,9 +116,6 @@
     <t>EmailVerificationToken</t>
   </si>
   <si>
-    <t>max 32, rejtett, null</t>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
@@ -798,6 +789,18 @@
   </si>
   <si>
     <t>Ezen a szinten a világtérképen milyen messze lévő városok ellen indítható ostrom.</t>
+  </si>
+  <si>
+    <t>ProfileImageUrl</t>
+  </si>
+  <si>
+    <t>A felhasználó által beállított profilkép webcíme. Ha még nem állított be profilképet, akkor az értéke null.</t>
+  </si>
+  <si>
+    <t>max 128</t>
+  </si>
+  <si>
+    <t>max 32, null</t>
   </si>
 </sst>
 </file>
@@ -1480,11 +1483,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FFD1A9D-9E14-4683-9B7B-AC97263CE9A8}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1511,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1544,7 +1547,7 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
@@ -1558,7 +1561,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.25">
@@ -1572,7 +1575,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1583,174 +1586,191 @@
         <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="6">
         <v>0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6" t="b">
         <v>0</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>253</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
+        <v>253</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-    </row>
-    <row r="16" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="11"/>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="A16:E16"/>
     <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -1782,7 +1802,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1791,7 +1811,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1817,7 +1837,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -1826,35 +1846,35 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1892,7 +1912,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1901,7 +1921,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1927,7 +1947,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -1936,29 +1956,29 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1996,7 +2016,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2005,7 +2025,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2031,7 +2051,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2040,35 +2060,35 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2106,7 +2126,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2115,7 +2135,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2141,7 +2161,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2150,60 +2170,60 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="78" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2241,7 +2261,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2250,7 +2270,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2276,7 +2296,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2285,170 +2305,170 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="29"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="29"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>240</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E17" s="29"/>
     </row>
@@ -2490,7 +2510,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2499,7 +2519,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2525,7 +2545,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2534,49 +2554,49 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2594,7 +2614,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -2610,7 +2630,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2619,7 +2639,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2645,7 +2665,7 @@
     </row>
     <row r="4" spans="1:5" ht="39.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2654,171 +2674,171 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="6">
         <v>100</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="6">
         <v>100</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="6">
         <v>100</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6">
         <v>50</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="6">
         <v>25</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="6">
         <v>0</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -2827,10 +2847,10 @@
     </row>
     <row r="17" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -2838,10 +2858,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -2849,10 +2869,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -2860,10 +2880,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -2889,7 +2909,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2905,7 +2925,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2914,7 +2934,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2940,7 +2960,7 @@
     </row>
     <row r="4" spans="1:5" ht="39.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2949,109 +2969,109 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -3060,10 +3080,10 @@
     </row>
     <row r="13" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -3071,10 +3091,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -3114,7 +3134,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3123,7 +3143,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -3149,7 +3169,7 @@
     </row>
     <row r="4" spans="1:5" ht="39.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -3158,35 +3178,35 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3198,7 +3218,7 @@
     </row>
     <row r="8" spans="1:5" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -3227,8 +3247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A36744-2979-45A2-9789-505325520E99}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -3244,7 +3264,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3253,7 +3273,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -3279,7 +3299,7 @@
     </row>
     <row r="4" spans="1:5" ht="39.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -3288,18 +3308,18 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
@@ -3310,50 +3330,50 @@
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="6">
         <v>0</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -3362,10 +3382,10 @@
     </row>
     <row r="11" spans="1:5" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
@@ -3404,7 +3424,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3413,7 +3433,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -3439,7 +3459,7 @@
     </row>
     <row r="4" spans="1:5" ht="39.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -3448,66 +3468,66 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="78" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="78" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -3516,10 +3536,10 @@
     </row>
     <row r="11" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>175</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>178</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
@@ -3527,10 +3547,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -3538,10 +3558,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -3582,7 +3602,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3591,7 +3611,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -3617,7 +3637,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -3626,55 +3646,55 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="78" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -3684,7 +3704,7 @@
     <row r="10" spans="1:5" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -3693,10 +3713,10 @@
     </row>
     <row r="12" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -3704,10 +3724,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -3748,7 +3768,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3757,7 +3777,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -3783,7 +3803,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -3792,12 +3812,12 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>10</v>
@@ -3806,116 +3826,116 @@
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3953,7 +3973,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3962,7 +3982,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -3988,7 +4008,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -3997,32 +4017,32 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Warehouse parameters added to database
</commit_message>
<xml_diff>
--- a/Docs/Adatbázis/Modellek gyűjteménye.xlsx
+++ b/Docs/Adatbázis/Modellek gyűjteménye.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\House of Swords\gameszko\Docs\Adatbázis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4695E6-2415-4385-B6D3-2D47B1477BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F50F631-57BD-4F8D-BC76-873E96EE2F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="260">
   <si>
     <t>User</t>
   </si>
@@ -801,6 +801,24 @@
   </si>
   <si>
     <t>max 32, null</t>
+  </si>
+  <si>
+    <t>BrigadeInWood</t>
+  </si>
+  <si>
+    <t>BrigadeInStone</t>
+  </si>
+  <si>
+    <t>BrigadeInMetal</t>
+  </si>
+  <si>
+    <t>BrigadeInGold</t>
+  </si>
+  <si>
+    <t>BrigadeInWarehouse</t>
+  </si>
+  <si>
+    <t>Ha az épület Warehouse típusú, akkor ezen értékek jelölik a nyersanyagtermelő helyekre küldött brigádok számát, illetve azokét, akik nem lettek elküldve sehova, így a raktárban maradtak.</t>
   </si>
 </sst>
 </file>
@@ -860,7 +878,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1102,11 +1120,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF23160F"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF23160F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF23160F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF23160F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF23160F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF23160F"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF23160F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF23160F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1194,6 +1249,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1485,7 +1549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FFD1A9D-9E14-4683-9B7B-AC97263CE9A8}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
@@ -2906,11 +2970,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9A3666-69F9-4F15-A5C6-4561FB99ADDC}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -3068,45 +3132,123 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
-    </row>
-    <row r="13" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B18" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="E11:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Trained Units tábla a barakkban toborzott egységek mentéséhez
</commit_message>
<xml_diff>
--- a/Docs/Adatbázis/Modellek gyűjteménye.xlsx
+++ b/Docs/Adatbázis/Modellek gyűjteménye.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\House of Swords\gameszko\Docs\Adatbázis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7963DE4E-0215-4463-8127-443068C4365C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56009EBC-C16A-4996-B100-820F34364288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="4" r:id="rId1"/>
@@ -20,14 +20,15 @@
     <sheet name="Bugreport" sheetId="11" r:id="rId5"/>
     <sheet name="Siege" sheetId="12" r:id="rId6"/>
     <sheet name="SiegingUnit" sheetId="13" r:id="rId7"/>
-    <sheet name="Unit" sheetId="15" r:id="rId8"/>
-    <sheet name="Levelstats_Church" sheetId="17" r:id="rId9"/>
-    <sheet name="Levelstats_Research" sheetId="18" r:id="rId10"/>
-    <sheet name="Levelstats_Market" sheetId="19" r:id="rId11"/>
-    <sheet name="Levelstats_Diplomacy" sheetId="20" r:id="rId12"/>
-    <sheet name="Levelstats_Infirmary" sheetId="21" r:id="rId13"/>
-    <sheet name="Levelstats_Warehouse" sheetId="23" r:id="rId14"/>
-    <sheet name="Levelstats_Barrack" sheetId="25" r:id="rId15"/>
+    <sheet name="TrainedUnit" sheetId="27" r:id="rId8"/>
+    <sheet name="Unit" sheetId="15" r:id="rId9"/>
+    <sheet name="Levelstats_Church" sheetId="17" r:id="rId10"/>
+    <sheet name="Levelstats_Research" sheetId="18" r:id="rId11"/>
+    <sheet name="Levelstats_Market" sheetId="19" r:id="rId12"/>
+    <sheet name="Levelstats_Diplomacy" sheetId="20" r:id="rId13"/>
+    <sheet name="Levelstats_Infirmary" sheetId="21" r:id="rId14"/>
+    <sheet name="Levelstats_Warehouse" sheetId="23" r:id="rId15"/>
+    <sheet name="Levelstats_Barrack" sheetId="25" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="276">
   <si>
     <t>User</t>
   </si>
@@ -578,15 +579,9 @@
     <t>SiegingUnits</t>
   </si>
   <si>
-    <t>$siegingUnits-&gt;siege</t>
-  </si>
-  <si>
     <t>Visszaadja az ostromot, melyben ez a támadó csapat vesz részt.</t>
   </si>
   <si>
-    <t>$siegingUnits-&gt;unitType</t>
-  </si>
-  <si>
     <t>Visszaadja ezen támadó egységek típusát.</t>
   </si>
   <si>
@@ -831,6 +826,48 @@
   </si>
   <si>
     <t>healedUnits</t>
+  </si>
+  <si>
+    <t>TrainedUnit</t>
+  </si>
+  <si>
+    <t>Egy városban toborzott egységtípus modelle. Tábla neve: trained_units.</t>
+  </si>
+  <si>
+    <t>TrainingID</t>
+  </si>
+  <si>
+    <t>town - 1:M - trained_units</t>
+  </si>
+  <si>
+    <t>units - 1:M - trained_units</t>
+  </si>
+  <si>
+    <t>A toborzás azonosítója.</t>
+  </si>
+  <si>
+    <t>Azon város azonosítója, melyben történt a toborzás. A város törlődése esetén kaszkádoltan törlődik a rekord.</t>
+  </si>
+  <si>
+    <t>$siegingUnit-&gt;siege</t>
+  </si>
+  <si>
+    <t>$siegingUnit-&gt;unitType</t>
+  </si>
+  <si>
+    <t>$trainedUnit-&gt;town</t>
+  </si>
+  <si>
+    <t>Visszaadja a várost, amelyben a toborzás történt.</t>
+  </si>
+  <si>
+    <t>Visszaadja a toborzott egységek típusát.</t>
+  </si>
+  <si>
+    <t>A toborzott egységek típusának azonosítója (pl. kardos, lovas, íjász). Az egység törlődése esetén kaszkádoltan törlődik a rekord.</t>
+  </si>
+  <si>
+    <t>A toborzott egységek száma.</t>
   </si>
 </sst>
 </file>
@@ -1662,7 +1699,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>15</v>
@@ -1730,7 +1767,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>25</v>
@@ -1747,7 +1784,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>25</v>
@@ -1761,7 +1798,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>25</v>
@@ -1775,7 +1812,7 @@
     </row>
     <row r="14" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>10</v>
@@ -1787,7 +1824,7 @@
         <v>25</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1854,6 +1891,113 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F847C7-0070-4297-8A99-4BFD8602DD31}">
+  <sheetPr>
+    <tabColor rgb="FFA6876E"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.42578125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="23.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:5" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8118204-6CD9-4398-8719-0B1F0C169CED}">
   <sheetPr>
     <tabColor rgb="FFA6876E"/>
@@ -1878,7 +2022,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1887,7 +2031,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1913,7 +2057,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -1922,12 +2066,12 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>19</v>
@@ -1936,12 +2080,12 @@
         <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -1950,7 +2094,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1963,7 +2107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3F54DE-E511-4BF3-B7F7-71FC66EB5BE6}">
   <sheetPr>
     <tabColor rgb="FFA6876E"/>
@@ -1988,7 +2132,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1997,7 +2141,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2023,7 +2167,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2032,29 +2176,29 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2067,7 +2211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BECF7C-8DA6-4B67-BB52-385623B94BBD}">
   <sheetPr>
     <tabColor rgb="FFA6876E"/>
@@ -2092,7 +2236,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2101,7 +2245,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2127,7 +2271,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2136,12 +2280,12 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>19</v>
@@ -2150,12 +2294,12 @@
         <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -2164,7 +2308,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2177,7 +2321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAC1367-C57E-428B-9657-D2C327792830}">
   <sheetPr>
     <tabColor rgb="FFA6876E"/>
@@ -2202,7 +2346,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2211,7 +2355,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2237,7 +2381,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2246,23 +2390,23 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>143</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="78" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -2271,12 +2415,12 @@
         <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>19</v>
@@ -2285,12 +2429,12 @@
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>19</v>
@@ -2299,7 +2443,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2312,7 +2456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23499FB7-7D6E-4D9B-ACAF-C5FB68718CE8}">
   <sheetPr>
     <tabColor rgb="FFA6876E"/>
@@ -2337,7 +2481,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2346,7 +2490,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2372,7 +2516,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2381,12 +2525,12 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>19</v>
@@ -2395,12 +2539,12 @@
         <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -2409,12 +2553,12 @@
         <v>20</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>19</v>
@@ -2426,7 +2570,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>19</v>
@@ -2438,7 +2582,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>19</v>
@@ -2450,7 +2594,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>19</v>
@@ -2459,12 +2603,12 @@
         <v>20</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>19</v>
@@ -2476,7 +2620,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>19</v>
@@ -2500,24 +2644,24 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>20</v>
@@ -2526,10 +2670,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>237</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>20</v>
@@ -2538,10 +2682,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>20</v>
@@ -2561,7 +2705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D931D9-2269-4E2C-ABF4-5F964AAA28C9}">
   <sheetPr>
     <tabColor rgb="FFA6876E"/>
@@ -2586,7 +2730,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2595,7 +2739,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2621,7 +2765,7 @@
     </row>
     <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2630,12 +2774,12 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>19</v>
@@ -2644,12 +2788,12 @@
         <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -2658,12 +2802,12 @@
         <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>19</v>
@@ -2672,7 +2816,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2984,7 +3128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9A3666-69F9-4F15-A5C6-4561FB99ADDC}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
@@ -3132,7 +3276,7 @@
         <v>72</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>25</v>
@@ -3146,7 +3290,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>19</v>
@@ -3158,12 +3302,12 @@
         <v>25</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>19</v>
@@ -3178,7 +3322,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>19</v>
@@ -3193,7 +3337,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>19</v>
@@ -3208,7 +3352,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>19</v>
@@ -3223,10 +3367,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>25</v>
@@ -3238,7 +3382,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>19</v>
@@ -3253,7 +3397,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>19</v>
@@ -3268,7 +3412,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>19</v>
@@ -3487,7 +3631,7 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -3599,7 +3743,7 @@
         <v>171</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
@@ -3718,7 +3862,7 @@
         <v>97</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>99</v>
@@ -3800,8 +3944,8 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:E9"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -3927,10 +4071,10 @@
     </row>
     <row r="12" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>179</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>180</v>
       </c>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -3938,10 +4082,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>181</v>
+        <v>270</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -3962,6 +4106,164 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027E0AF9-1785-41F2-8DF7-CF43FA767097}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="23.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:5" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB58D31-F175-41FC-8BBC-87088CA0323D}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -4096,7 +4398,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="39" x14ac:dyDescent="0.25">
@@ -4150,113 +4452,6 @@
       </c>
       <c r="E13" s="5" t="s">
         <v>150</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F847C7-0070-4297-8A99-4BFD8602DD31}">
-  <sheetPr>
-    <tabColor rgb="FFA6876E"/>
-  </sheetPr>
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="D8" sqref="D8"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.42578125" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="23.7109375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="3" spans="1:5" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>